<commit_message>
Refactored tests, updated selectors to use selenium specific identifiers, updated README
</commit_message>
<xml_diff>
--- a/src/test/resources/Wazoku_TestData.xlsx
+++ b/src/test/resources/Wazoku_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\eclipse\WazokuAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE954DD-1413-4A2B-A66C-3EABF949D6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D1F8B3-CD09-462D-9F84-832591618F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{033A79BE-225D-4BB0-99FD-41FD053167B3}"/>
   </bookViews>
@@ -430,14 +430,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>